<commit_message>
update with fuzzy match
</commit_message>
<xml_diff>
--- a/data/interim/fuzzy_matches.xlsx
+++ b/data/interim/fuzzy_matches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/DataVisualizations/asbestos-dashboard/asbestos-dashboard-data/data/interim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9EAFD5-71A8-BE41-AB72-13080DB6A1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76441BD1-073B-0847-A8F8-999732C6D30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>facility_name</t>
   </si>
@@ -40,37 +40,19 @@
     <t>match</t>
   </si>
   <si>
-    <t>Richard R Wright Elementary School</t>
-  </si>
-  <si>
-    <t>Richard R. Wright School</t>
-  </si>
-  <si>
-    <t>2700 W DAUPHIN ST</t>
-  </si>
-  <si>
-    <t>2201 N 28TH ST</t>
+    <t>PSD Cassidy Elementary School</t>
+  </si>
+  <si>
+    <t>Kenderton Elementary School</t>
+  </si>
+  <si>
+    <t>6523-43 LANSDOWNE AVE Lewis C. Cassidy Elementary School</t>
+  </si>
+  <si>
+    <t>1500 W ONTARIO ST</t>
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>FS Edmonds School</t>
-  </si>
-  <si>
-    <t>Franklin S. Edmonds School</t>
-  </si>
-  <si>
-    <t>8060 WILLIAMS AVE</t>
-  </si>
-  <si>
-    <t>8025 THOURON AVE</t>
-  </si>
-  <si>
-    <t>PIERCE ES @ PRATT BUILDING</t>
-  </si>
-  <si>
-    <t>2200 N 22ND ST</t>
   </si>
 </sst>
 </file>
@@ -89,7 +71,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -434,18 +415,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -482,40 +461,9 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>0.81</v>
+        <v>0.68</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>0.81</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update with fuzzy matches
</commit_message>
<xml_diff>
--- a/data/interim/fuzzy_matches.xlsx
+++ b/data/interim/fuzzy_matches.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/DataVisualizations/asbestos-dashboard/asbestos-dashboard-data/data/interim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76441BD1-073B-0847-A8F8-999732C6D30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE8E051-8C54-A44F-92FD-3EEF046896DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,13 +40,13 @@
     <t>match</t>
   </si>
   <si>
-    <t>PSD Cassidy Elementary School</t>
+    <t>MAYFAIR ELEMENTARY SCHOOL</t>
   </si>
   <si>
     <t>Kenderton Elementary School</t>
   </si>
   <si>
-    <t>6523-43 LANSDOWNE AVE Lewis C. Cassidy Elementary School</t>
+    <t>2901 PRINCETON AVE</t>
   </si>
   <si>
     <t>1500 W ONTARIO ST</t>
@@ -71,6 +71,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -423,8 +424,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -461,7 +466,7 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>0.68</v>
+        <v>0.73</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>

</xml_diff>